<commit_message>
added business_plan_development.pptx added milestones into development_plan.xlsx
</commit_message>
<xml_diff>
--- a/docs/products/development_plan.xlsx
+++ b/docs/products/development_plan.xlsx
@@ -89,184 +89,6 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Dong Zhao</author>
-  </authors>
-  <commentList>
-    <comment ref="F3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Dong Zhao:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Milestone #1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #4</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #5</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #6</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dong Zhao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Milestone #7</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="145">
   <si>
@@ -709,7 +531,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,19 +636,6 @@
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -933,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1143,13 +952,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1346,6 +1168,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1627,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2988,7 +2813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3187,40 +3012,40 @@
       <c r="C3" s="56"/>
       <c r="D3" s="64"/>
       <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
+      <c r="F3" s="66"/>
       <c r="G3" s="65"/>
       <c r="H3" s="65"/>
       <c r="I3" s="65"/>
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
       <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
+      <c r="M3" s="66"/>
       <c r="N3" s="65"/>
       <c r="O3" s="65"/>
       <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
+      <c r="Q3" s="66"/>
       <c r="R3" s="65"/>
       <c r="S3" s="65"/>
       <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
+      <c r="U3" s="66"/>
       <c r="V3" s="65"/>
       <c r="W3" s="65"/>
       <c r="X3" s="65"/>
       <c r="Y3" s="65"/>
       <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
+      <c r="AA3" s="66"/>
       <c r="AB3" s="65"/>
       <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
+      <c r="AD3" s="66"/>
       <c r="AE3" s="65"/>
       <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
+      <c r="AG3" s="66"/>
       <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AI3" s="66"/>
       <c r="AJ3" s="65"/>
-      <c r="AK3" s="65"/>
+      <c r="AK3" s="66"/>
       <c r="AL3" s="65"/>
-      <c r="AM3" s="65"/>
+      <c r="AM3" s="66"/>
       <c r="AN3" s="65"/>
       <c r="AO3" s="65"/>
     </row>
@@ -3705,6 +3530,5 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>